<commit_message>
Check in code mainly for EEPROM. 	- PORT1/2/3/4 PORT_OTA 4 bytes of uint8_t 	- APN 32 bytes 	- Removed # from EEPROM string
</commit_message>
<xml_diff>
--- a/DOC/spec/EEPROMMap.xlsx
+++ b/DOC/spec/EEPROMMap.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Page 0 EEPROM Map" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="124">
   <si>
     <t xml:space="preserve">Add \ Byte</t>
   </si>
@@ -69,133 +69,133 @@
     <t xml:space="preserve">0x20</t>
   </si>
   <si>
+    <t xml:space="preserve">0x30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01# IP1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x04</t>
+  </si>
+  <si>
     <t xml:space="preserve">reserved2</t>
   </si>
   <si>
-    <t xml:space="preserve">0x30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01# IP1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0x04</t>
+    <t xml:space="preserve">0x50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02# IP2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x60</t>
   </si>
   <si>
     <t xml:space="preserve">reserved3</t>
   </si>
   <si>
-    <t xml:space="preserve">0x50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">02# IP2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0x60</t>
+    <t xml:space="preserve">0x70</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03# IP3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x80</t>
   </si>
   <si>
     <t xml:space="preserve">reserved4</t>
   </si>
   <si>
-    <t xml:space="preserve">0x70</t>
-  </si>
-  <si>
-    <t xml:space="preserve">03# IP3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0x80</t>
+    <t xml:space="preserve">0x90</t>
+  </si>
+  <si>
+    <t xml:space="preserve">04# IP4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0xA0</t>
   </si>
   <si>
     <t xml:space="preserve">reserved5</t>
   </si>
   <si>
-    <t xml:space="preserve">0x90</t>
-  </si>
-  <si>
-    <t xml:space="preserve">04# IP4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0xA0</t>
+    <t xml:space="preserve">31#  PORT1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">32#  PORT2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0xB0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">33#  PORT3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">34#  PORT4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">09#</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12#</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13#</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14#</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15#</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16#</t>
   </si>
   <si>
     <t xml:space="preserve">reserved6</t>
   </si>
   <si>
-    <t xml:space="preserve">0xB0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">31#  PORT1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">32#  PORT2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">33# PORT3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">34# PORT4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">09#</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12#</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13#</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14#</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15#</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16#</t>
+    <t xml:space="preserve">0xC0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">05# Access Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">06#</t>
+  </si>
+  <si>
+    <t xml:space="preserve">07#</t>
+  </si>
+  <si>
+    <t xml:space="preserve">08#</t>
   </si>
   <si>
     <t xml:space="preserve">reserved7</t>
   </si>
   <si>
-    <t xml:space="preserve">0xC0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">05# Access Code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">06#</t>
-  </si>
-  <si>
-    <t xml:space="preserve">07#</t>
-  </si>
-  <si>
-    <t xml:space="preserve">08#</t>
+    <t xml:space="preserve">0xD0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10# Unit Account</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reserved8 11# Line Card</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11# Line Card</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0xE0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#95</t>
   </si>
   <si>
     <t xml:space="preserve">reserved8</t>
   </si>
   <si>
-    <t xml:space="preserve">0xD0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10# Unit Account</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reserved8 11# Line Card</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11# Line Card</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0xE0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#95</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reserved9</t>
-  </si>
-  <si>
     <t xml:space="preserve">0xF0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHECKSUM</t>
   </si>
   <si>
     <t xml:space="preserve">FR First Run – used to check if we need init EEPROM</t>
@@ -408,6 +408,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -425,29 +426,34 @@
       <family val="0"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <b val="true"/>
-      <sz val="24"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF333333"/>
+      <color rgb="FFCC0000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <i val="true"/>
@@ -455,6 +461,36 @@
       <color rgb="FF808080"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF006600"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="24"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <u val="single"/>
@@ -462,56 +498,35 @@
       <color rgb="FF0000EE"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF006600"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF996600"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FFCC0000"/>
+      <color rgb="FF333333"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFC9211E"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="12">
@@ -520,30 +535,6 @@
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCFFCC"/>
-        <bgColor rgb="FFCCFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCCCC"/>
-        <bgColor rgb="FFDDDDDD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCC0000"/>
-        <bgColor rgb="FFC9211E"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -561,6 +552,30 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFDDDDDD"/>
         <bgColor rgb="FFFFCCCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCCC"/>
+        <bgColor rgb="FFDDDDDD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC0000"/>
+        <bgColor rgb="FFC9211E"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
@@ -637,55 +652,55 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="8" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
@@ -734,8 +749,8 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -802,23 +817,23 @@
     <cellStyle name="Currency" xfId="17" builtinId="4"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
-    <cellStyle name="Heading" xfId="20"/>
-    <cellStyle name="Heading 1" xfId="21"/>
-    <cellStyle name="Heading 2" xfId="22"/>
-    <cellStyle name="Text" xfId="23"/>
-    <cellStyle name="Note" xfId="24"/>
-    <cellStyle name="Footnote" xfId="25"/>
-    <cellStyle name="Hyperlink" xfId="26"/>
-    <cellStyle name="Status" xfId="27"/>
-    <cellStyle name="Good" xfId="28"/>
-    <cellStyle name="Neutral" xfId="29"/>
-    <cellStyle name="Bad" xfId="30"/>
-    <cellStyle name="Warning" xfId="31"/>
-    <cellStyle name="Error" xfId="32"/>
-    <cellStyle name="Accent" xfId="33"/>
-    <cellStyle name="Accent 1" xfId="34"/>
-    <cellStyle name="Accent 2" xfId="35"/>
-    <cellStyle name="Accent 3" xfId="36"/>
+    <cellStyle name="Accent 1 17" xfId="20"/>
+    <cellStyle name="Accent 16" xfId="21"/>
+    <cellStyle name="Accent 2 18" xfId="22"/>
+    <cellStyle name="Accent 3 19" xfId="23"/>
+    <cellStyle name="Bad 13" xfId="24"/>
+    <cellStyle name="Error 15" xfId="25"/>
+    <cellStyle name="Footnote 8" xfId="26"/>
+    <cellStyle name="Good 11" xfId="27"/>
+    <cellStyle name="Heading 1 4" xfId="28"/>
+    <cellStyle name="Heading 2 5" xfId="29"/>
+    <cellStyle name="Heading 3" xfId="30"/>
+    <cellStyle name="Hyperlink 9" xfId="31"/>
+    <cellStyle name="Neutral 12" xfId="32"/>
+    <cellStyle name="Note 7" xfId="33"/>
+    <cellStyle name="Status 10" xfId="34"/>
+    <cellStyle name="Text 6" xfId="35"/>
+    <cellStyle name="Warning 14" xfId="36"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -890,8 +905,8 @@
   </sheetPr>
   <dimension ref="A1:R34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B28" activeCellId="0" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1010,31 +1025,29 @@
       <c r="A4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
-      <c r="M4" s="8"/>
-      <c r="N4" s="8"/>
-      <c r="O4" s="8"/>
-      <c r="P4" s="8"/>
-      <c r="Q4" s="8"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="7"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>16</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>17</v>
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
@@ -1054,10 +1067,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>18</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>19</v>
       </c>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
@@ -1077,10 +1090,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>20</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>21</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -1100,10 +1113,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="6" t="s">
         <v>22</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>23</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
@@ -1123,10 +1136,10 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>24</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>25</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -1146,10 +1159,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>26</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>27</v>
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
@@ -1169,10 +1182,10 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="5" t="s">
         <v>28</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>29</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
@@ -1192,10 +1205,10 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>30</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>31</v>
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
@@ -1204,64 +1217,64 @@
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="6"/>
-      <c r="M12" s="6"/>
-      <c r="N12" s="6"/>
-      <c r="O12" s="6"/>
-      <c r="P12" s="6"/>
-      <c r="Q12" s="6"/>
+      <c r="J12" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="O12" s="5"/>
+      <c r="P12" s="5"/>
+      <c r="Q12" s="5"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C13" s="5"/>
-      <c r="D13" s="5" t="s">
-        <v>34</v>
-      </c>
+      <c r="D13" s="5"/>
       <c r="E13" s="5"/>
       <c r="F13" s="5" t="s">
         <v>35</v>
       </c>
       <c r="G13" s="5"/>
-      <c r="H13" s="5" t="s">
-        <v>36</v>
-      </c>
+      <c r="H13" s="5"/>
       <c r="I13" s="5"/>
       <c r="J13" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K13" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="K13" s="5" t="s">
+      <c r="L13" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="L13" s="5" t="s">
+      <c r="M13" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="M13" s="5" t="s">
+      <c r="N13" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="N13" s="5" t="s">
+      <c r="O13" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="O13" s="5" t="s">
+      <c r="P13" s="6" t="s">
         <v>42</v>
-      </c>
-      <c r="P13" s="6" t="s">
-        <v>43</v>
       </c>
       <c r="Q13" s="6"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>44</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>45</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
@@ -1270,16 +1283,16 @@
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
       <c r="I14" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="J14" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="J14" s="5" t="s">
+      <c r="K14" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="K14" s="5" t="s">
+      <c r="L14" s="6" t="s">
         <v>48</v>
-      </c>
-      <c r="L14" s="6" t="s">
-        <v>49</v>
       </c>
       <c r="M14" s="6"/>
       <c r="N14" s="6"/>
@@ -1289,22 +1302,22 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>50</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>51</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
       <c r="G15" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
       <c r="J15" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K15" s="9"/>
       <c r="L15" s="9"/>
@@ -1316,71 +1329,71 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B16" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="C16" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="C16" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
-      <c r="K16" s="6"/>
-      <c r="L16" s="6"/>
-      <c r="M16" s="6"/>
-      <c r="N16" s="6"/>
-      <c r="O16" s="6"/>
-      <c r="P16" s="6"/>
-      <c r="Q16" s="6"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="8"/>
+      <c r="O16" s="8"/>
+      <c r="P16" s="11"/>
+      <c r="Q16" s="11"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17" s="6"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="8"/>
+      <c r="N17" s="8"/>
+      <c r="O17" s="8"/>
+      <c r="P17" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B17" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="6"/>
-      <c r="K17" s="6"/>
-      <c r="L17" s="6"/>
-      <c r="M17" s="6"/>
-      <c r="N17" s="6"/>
-      <c r="O17" s="6"/>
-      <c r="P17" s="6"/>
-      <c r="Q17" s="6"/>
+      <c r="Q17" s="5"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="11" t="s">
+      <c r="B21" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="11"/>
-      <c r="J21" s="11"/>
-      <c r="K21" s="11"/>
-      <c r="L21" s="11"/>
-      <c r="M21" s="11"/>
-      <c r="N21" s="11"/>
-      <c r="O21" s="11"/>
-      <c r="P21" s="11"/>
-      <c r="Q21" s="11"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="12"/>
+      <c r="K21" s="12"/>
+      <c r="L21" s="12"/>
+      <c r="M21" s="12"/>
+      <c r="N21" s="12"/>
+      <c r="O21" s="12"/>
+      <c r="P21" s="12"/>
+      <c r="Q21" s="12"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="12" t="s">
@@ -1672,8 +1685,7 @@
   <mergeCells count="37">
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="G2:P2"/>
-    <mergeCell ref="B3:Q3"/>
-    <mergeCell ref="B4:Q4"/>
+    <mergeCell ref="B3:Q4"/>
     <mergeCell ref="B5:Q5"/>
     <mergeCell ref="B6:Q6"/>
     <mergeCell ref="B7:Q7"/>
@@ -1681,18 +1693,19 @@
     <mergeCell ref="B9:Q9"/>
     <mergeCell ref="B10:Q10"/>
     <mergeCell ref="B11:Q11"/>
-    <mergeCell ref="B12:Q12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="B12:I12"/>
+    <mergeCell ref="J12:M12"/>
+    <mergeCell ref="N12:Q12"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="F13:I13"/>
     <mergeCell ref="P13:Q13"/>
     <mergeCell ref="B14:H14"/>
     <mergeCell ref="L14:Q14"/>
     <mergeCell ref="B15:I15"/>
     <mergeCell ref="J15:Q15"/>
-    <mergeCell ref="C16:Q16"/>
-    <mergeCell ref="B17:Q17"/>
+    <mergeCell ref="C16:O17"/>
+    <mergeCell ref="P16:Q16"/>
+    <mergeCell ref="P17:Q17"/>
     <mergeCell ref="B21:Q21"/>
     <mergeCell ref="B22:Q22"/>
     <mergeCell ref="B23:Q23"/>
@@ -1725,8 +1738,8 @@
   </sheetPr>
   <dimension ref="A1:Q20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P17" activeCellId="0" sqref="P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1890,7 +1903,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>78</v>
@@ -1956,7 +1969,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>83</v>
@@ -1989,7 +2002,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>85</v>
@@ -2022,7 +2035,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>87</v>
@@ -2055,7 +2068,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>10</v>
@@ -2078,7 +2091,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
@@ -2099,7 +2112,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
@@ -2120,7 +2133,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
@@ -2141,7 +2154,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
@@ -2162,7 +2175,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>89</v>
@@ -2185,10 +2198,10 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
@@ -2208,17 +2221,19 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>90</v>
       </c>
       <c r="C17" s="5"/>
-      <c r="D17" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
+      <c r="D17" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E17" s="5"/>
+      <c r="F17" s="6" t="s">
+        <v>22</v>
+      </c>
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
@@ -2228,8 +2243,10 @@
       <c r="M17" s="6"/>
       <c r="N17" s="6"/>
       <c r="O17" s="6"/>
-      <c r="P17" s="6"/>
-      <c r="Q17" s="6"/>
+      <c r="P17" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q17" s="5"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="12" t="s">
@@ -2254,7 +2271,7 @@
       <c r="Q20" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="22">
+  <mergeCells count="23">
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="J2:O2"/>
     <mergeCell ref="B3:G3"/>
@@ -2274,8 +2291,9 @@
     <mergeCell ref="B10:Q14"/>
     <mergeCell ref="B15:Q15"/>
     <mergeCell ref="B16:Q16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:Q17"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="F17:O17"/>
+    <mergeCell ref="P17:Q17"/>
     <mergeCell ref="B20:Q20"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2295,8 +2313,8 @@
   </sheetPr>
   <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H40" activeCellId="0" sqref="H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2606,7 +2624,7 @@
         <v>2</v>
       </c>
       <c r="C22" s="20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D22" s="21" t="s">
         <v>113</v>
@@ -2620,7 +2638,7 @@
       </c>
       <c r="B23" s="23"/>
       <c r="C23" s="20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D23" s="21"/>
       <c r="E23" s="24"/>

</xml_diff>

<commit_message>
Check in the code using page0_eeprom data. But AT+CGDCONT error - not sure what's wrong with it.
AT+CGDCONT=3,"IP","11583.mcs"

+CME ERROR: operation not allowed
</commit_message>
<xml_diff>
--- a/DOC/spec/EEPROMMap.xlsx
+++ b/DOC/spec/EEPROMMap.xlsx
@@ -5,12 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Page 0 EEPROM Map" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Page 1 EEPROM Map" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="stack_buffer structure" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="resp_buffer" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="123">
   <si>
     <t xml:space="preserve">Add \ Byte</t>
   </si>
@@ -75,7 +76,7 @@
     <t xml:space="preserve">01# IP1</t>
   </si>
   <si>
-    <t xml:space="preserve">0x04</t>
+    <t xml:space="preserve">0x40</t>
   </si>
   <si>
     <t xml:space="preserve">reserved2</t>
@@ -262,9 +263,6 @@
   </si>
   <si>
     <t xml:space="preserve">48#</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0x40</t>
   </si>
   <si>
     <t xml:space="preserve">49#</t>
@@ -408,7 +406,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -426,11 +423,68 @@
       <family val="0"/>
     </font>
     <font>
+      <b val="true"/>
+      <sz val="24"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <color rgb="FF808080"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="10"/>
+      <color rgb="FF0000EE"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF006600"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF996600"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFCC0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -438,95 +492,24 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FFCC0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <i val="true"/>
-      <sz val="10"/>
-      <color rgb="FF808080"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF006600"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="24"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <u val="single"/>
-      <sz val="10"/>
-      <color rgb="FF0000EE"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF996600"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF333333"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFC9211E"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="12">
@@ -535,6 +518,30 @@
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCCC"/>
+        <bgColor rgb="FFDDDDDD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC0000"/>
+        <bgColor rgb="FFC9211E"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -552,30 +559,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFDDDDDD"/>
         <bgColor rgb="FFFFCCCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCCCC"/>
-        <bgColor rgb="FFDDDDDD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCC0000"/>
-        <bgColor rgb="FFC9211E"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCFFCC"/>
-        <bgColor rgb="FFCCFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
@@ -628,7 +611,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="37">
+  <cellStyleXfs count="54">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -652,46 +635,97 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
     <xf numFmtId="164" fontId="14" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="8" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -700,7 +734,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
@@ -810,30 +844,47 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="40">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Comma" xfId="15" builtinId="3"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
     <cellStyle name="Currency" xfId="17" builtinId="4"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
-    <cellStyle name="Accent 1 17" xfId="20"/>
-    <cellStyle name="Accent 16" xfId="21"/>
-    <cellStyle name="Accent 2 18" xfId="22"/>
-    <cellStyle name="Accent 3 19" xfId="23"/>
-    <cellStyle name="Bad 13" xfId="24"/>
-    <cellStyle name="Error 15" xfId="25"/>
-    <cellStyle name="Footnote 8" xfId="26"/>
-    <cellStyle name="Good 11" xfId="27"/>
-    <cellStyle name="Heading 1 4" xfId="28"/>
-    <cellStyle name="Heading 2 5" xfId="29"/>
-    <cellStyle name="Heading 3" xfId="30"/>
-    <cellStyle name="Hyperlink 9" xfId="31"/>
-    <cellStyle name="Neutral 12" xfId="32"/>
-    <cellStyle name="Note 7" xfId="33"/>
-    <cellStyle name="Status 10" xfId="34"/>
-    <cellStyle name="Text 6" xfId="35"/>
-    <cellStyle name="Warning 14" xfId="36"/>
+    <cellStyle name="Heading" xfId="20"/>
+    <cellStyle name="Heading 1" xfId="21"/>
+    <cellStyle name="Heading 2" xfId="22"/>
+    <cellStyle name="Text" xfId="23"/>
+    <cellStyle name="Note" xfId="24"/>
+    <cellStyle name="Footnote" xfId="25"/>
+    <cellStyle name="Hyperlink" xfId="26"/>
+    <cellStyle name="Status" xfId="27"/>
+    <cellStyle name="Good" xfId="28"/>
+    <cellStyle name="Neutral" xfId="29"/>
+    <cellStyle name="Bad" xfId="30"/>
+    <cellStyle name="Warning" xfId="31"/>
+    <cellStyle name="Error" xfId="32"/>
+    <cellStyle name="Accent" xfId="33"/>
+    <cellStyle name="Accent 1" xfId="34"/>
+    <cellStyle name="Accent 2" xfId="35"/>
+    <cellStyle name="Accent 3" xfId="36"/>
+    <cellStyle name="Accent 1 17" xfId="37"/>
+    <cellStyle name="Accent 16" xfId="38"/>
+    <cellStyle name="Accent 2 18" xfId="39"/>
+    <cellStyle name="Accent 3 19" xfId="40"/>
+    <cellStyle name="Bad 13" xfId="41"/>
+    <cellStyle name="Error 15" xfId="42"/>
+    <cellStyle name="Footnote 8" xfId="43"/>
+    <cellStyle name="Good 11" xfId="44"/>
+    <cellStyle name="Heading 1 4" xfId="45"/>
+    <cellStyle name="Heading 2 5" xfId="46"/>
+    <cellStyle name="Heading 3" xfId="47"/>
+    <cellStyle name="Hyperlink 9" xfId="48"/>
+    <cellStyle name="Neutral 12" xfId="49"/>
+    <cellStyle name="Note 7" xfId="50"/>
+    <cellStyle name="Status 10" xfId="51"/>
+    <cellStyle name="Text 6" xfId="52"/>
+    <cellStyle name="Warning 14" xfId="53"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -905,8 +956,8 @@
   </sheetPr>
   <dimension ref="A1:R34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B28" activeCellId="0" sqref="B28"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1936,10 +1987,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>80</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>81</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -1953,7 +2004,7 @@
         <v>0</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K6" s="5"/>
       <c r="L6" s="5"/>
@@ -1972,7 +2023,7 @@
         <v>19</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -1986,7 +2037,7 @@
         <v>0</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
@@ -2005,7 +2056,7 @@
         <v>21</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -2019,7 +2070,7 @@
         <v>0</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
@@ -2038,7 +2089,7 @@
         <v>23</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -2052,7 +2103,7 @@
         <v>0</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K9" s="5"/>
       <c r="L9" s="5"/>
@@ -2178,7 +2229,7 @@
         <v>49</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
@@ -2224,7 +2275,7 @@
         <v>56</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="5" t="s">
@@ -2250,7 +2301,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C20" s="12" t="s">
         <v>60</v>
@@ -2330,22 +2381,22 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="D1" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="E1" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="F1" s="19" t="s">
         <v>96</v>
-      </c>
-      <c r="F1" s="19" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2356,16 +2407,16 @@
         <v>1</v>
       </c>
       <c r="C2" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="D2" s="21" t="s">
         <v>98</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="E2" s="22" t="s">
         <v>99</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="F2" s="5" t="s">
         <v>100</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2376,14 +2427,14 @@
         <v>1</v>
       </c>
       <c r="C3" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="D3" s="21" t="s">
         <v>102</v>
-      </c>
-      <c r="D3" s="21" t="s">
-        <v>103</v>
       </c>
       <c r="E3" s="22"/>
       <c r="F3" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2394,14 +2445,14 @@
         <v>1</v>
       </c>
       <c r="C4" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="D4" s="21" t="s">
         <v>105</v>
-      </c>
-      <c r="D4" s="21" t="s">
-        <v>106</v>
       </c>
       <c r="E4" s="22"/>
       <c r="F4" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2412,14 +2463,14 @@
         <v>1</v>
       </c>
       <c r="C5" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="D5" s="21" t="s">
         <v>107</v>
-      </c>
-      <c r="D5" s="21" t="s">
-        <v>108</v>
       </c>
       <c r="E5" s="22"/>
       <c r="F5" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2430,14 +2481,14 @@
         <v>1</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D6" s="21" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E6" s="22"/>
       <c r="F6" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2451,13 +2502,13 @@
         <v>3</v>
       </c>
       <c r="D7" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="E7" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="E7" s="22" t="s">
-        <v>111</v>
-      </c>
       <c r="F7" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2469,13 +2520,13 @@
         <v>3</v>
       </c>
       <c r="D8" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="E8" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="E8" s="22" t="s">
-        <v>111</v>
-      </c>
       <c r="F8" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2490,10 +2541,10 @@
       </c>
       <c r="D9" s="8"/>
       <c r="E9" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2627,7 +2678,7 @@
         <v>15</v>
       </c>
       <c r="D22" s="21" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E22" s="24"/>
       <c r="F22" s="5"/>
@@ -2655,13 +2706,13 @@
         <v>7548</v>
       </c>
       <c r="D24" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="E24" s="22" t="s">
         <v>114</v>
       </c>
-      <c r="E24" s="22" t="s">
-        <v>115</v>
-      </c>
       <c r="F24" s="25" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2702,12 +2753,12 @@
         <v>1</v>
       </c>
       <c r="C28" s="20" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D28" s="21"/>
       <c r="E28" s="22"/>
       <c r="F28" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2721,13 +2772,13 @@
         <v>4007</v>
       </c>
       <c r="D29" s="21" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E29" s="22" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2768,14 +2819,14 @@
         <v>9</v>
       </c>
       <c r="C33" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="D33" s="21" t="s">
         <v>118</v>
-      </c>
-      <c r="D33" s="21" t="s">
-        <v>119</v>
       </c>
       <c r="E33" s="24"/>
       <c r="F33" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2867,11 +2918,11 @@
       </c>
       <c r="C42" s="20"/>
       <c r="D42" s="21" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E42" s="22"/>
       <c r="F42" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2883,11 +2934,11 @@
       </c>
       <c r="C43" s="20"/>
       <c r="D43" s="21" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E43" s="22"/>
       <c r="F43" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2897,11 +2948,11 @@
       <c r="B44" s="23"/>
       <c r="C44" s="20"/>
       <c r="D44" s="21" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E44" s="22"/>
       <c r="F44" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2912,14 +2963,14 @@
         <v>1</v>
       </c>
       <c r="C45" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="D45" s="21" t="s">
         <v>122</v>
-      </c>
-      <c r="D45" s="21" t="s">
-        <v>123</v>
       </c>
       <c r="E45" s="22"/>
       <c r="F45" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -2957,4 +3008,30 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+  </cols>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>